<commit_message>
tarificator : correction bug et ajout de la prise en charge de remise multiple
</commit_message>
<xml_diff>
--- a/rem_fam.xlsx
+++ b/rem_fam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.38.161\Donnees_AUS\Utilisateurs AUSCHITZKY\CAIL\test TARIFICATOR\VERSIONS\VERSION7.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F7CBD1-1DCB-4BE2-8BB3-2C563DE99A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D111ACBA-C70F-4A8A-BE0F-61C80A2213EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{AB818483-2D10-439E-85CA-0BAFE6535C47}"/>
   </bookViews>
@@ -2936,8 +2936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0107CBC-83A2-4E51-BF84-355C099711AB}">
   <dimension ref="A1:I939"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C750" sqref="C750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>